<commit_message>
Minor alterations of heatmaps and italicizing gene names
</commit_message>
<xml_diff>
--- a/CF39vsCF39S/Pure Temperature Analysis Comparisons/Individual Heatmaps/Raw Unmodified individual Data.xlsx
+++ b/CF39vsCF39S/Pure Temperature Analysis Comparisons/Individual Heatmaps/Raw Unmodified individual Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flagella" sheetId="1" r:id="rId1"/>
@@ -24,18 +24,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="62">
   <si>
-    <t>TssA1</t>
-  </si>
-  <si>
-    <t>TssC1</t>
-  </si>
-  <si>
-    <t>Hcp1</t>
-  </si>
-  <si>
-    <t>ClpV1</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -208,6 +196,18 @@
   </si>
   <si>
     <t>PROKKA_05246_sense</t>
+  </si>
+  <si>
+    <t>tssA1</t>
+  </si>
+  <si>
+    <t>tssC1</t>
+  </si>
+  <si>
+    <t>hcp1</t>
+  </si>
+  <si>
+    <t>clpV1</t>
   </si>
 </sst>
 </file>
@@ -584,85 +584,85 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
         <v>-2.805132899065002</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>-1.8506441211717566</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
         <v>-2.1693277459558882</v>
@@ -671,90 +671,90 @@
         <v>-7.0839198395372165</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>-12.560055533504462</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
         <v>-2.7829721356708945</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1">
         <v>-6.6665742518813138</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E8" s="3">
         <v>-1.8229156542115235</v>
@@ -763,168 +763,168 @@
         <v>-12.428351537006888</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1">
         <v>-2.4417773387254424</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>-2.0957685469823528</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>-2.0072968655914454</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>-2.7859769929715092</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>-2.5491930795998945</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>-2.6479047446915573</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>-2.3336947784548681</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -936,47 +936,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>-2.1307327690469124</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>1.8922026508731662</v>
@@ -985,21 +985,21 @@
         <v>2.3026647981748942</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>-1.884527605151143</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>2.165097821572759</v>
@@ -1008,53 +1008,53 @@
         <v>2.0132088462653983</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
         <v>2.4919797765040346</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>2.0458105977734329</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:L1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,30 +1085,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>-1.9486733330704638</v>
@@ -1117,58 +1117,58 @@
         <v>-2.4349707518613628</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>-2.3016392763262234</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>-2.1878483751500197</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>-1.8981661680730593</v>
@@ -1177,18 +1177,18 @@
         <v>-2.2368711484856916</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
         <v>-1.8229387885065877</v>
@@ -1197,87 +1197,87 @@
         <v>-2.3996221696332598</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
         <v>-10.919346729820377</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
         <v>-6.4367603038960004</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
         <v>-9.7665782447009146</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
         <v>-2.8824840628634636</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
         <v>-2.9075520935040018</v>
@@ -1285,16 +1285,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>-1.8713690641270391</v>
@@ -1324,117 +1324,117 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>-2.1093170022393029</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
         <v>-5.1527322310062997</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
         <v>3.8995685999865501</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>5.3102654012313604</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>